<commit_message>
casecade & move cmd
add joint limit
       case cade control
        move join cmd
</commit_message>
<xml_diff>
--- a/protocol.xlsx
+++ b/protocol.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pienapat/Documents/GitHub/Manipulator_lowlevel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39081069-6AEC-0E45-B0F5-BCACD75E43B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4EECDE1-05E2-1B43-8DF1-F5D10F81A9D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15760" xr2:uid="{521507E1-042C-C644-B1F6-1B5E6F45BA0E}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15760" activeTab="1" xr2:uid="{521507E1-042C-C644-B1F6-1B5E6F45BA0E}"/>
   </bookViews>
   <sheets>
     <sheet name="command pack" sheetId="1" r:id="rId1"/>
     <sheet name="ack err" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,6 +28,7 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="100">
   <si>
     <t>header</t>
   </si>
@@ -184,9 +185,6 @@
     <t>request Chessboard encoder</t>
   </si>
   <si>
-    <t>0xFE</t>
-  </si>
-  <si>
     <t>ang_h</t>
   </si>
   <si>
@@ -223,12 +221,6 @@
     <t>checksum error</t>
   </si>
   <si>
-    <t>0xEA</t>
-  </si>
-  <si>
-    <t>0xEB</t>
-  </si>
-  <si>
     <t>bits</t>
   </si>
   <si>
@@ -311,6 +303,39 @@
   </si>
   <si>
     <t>checksum = ~( (sum(parameter) + length + instruction) &amp; 0xFF )</t>
+  </si>
+  <si>
+    <t>0x51</t>
+  </si>
+  <si>
+    <t>0x52</t>
+  </si>
+  <si>
+    <t>manipulators position</t>
+  </si>
+  <si>
+    <t>0xA5</t>
+  </si>
+  <si>
+    <t>manipulator position</t>
+  </si>
+  <si>
+    <t>0xA6</t>
+  </si>
+  <si>
+    <t>0x60</t>
+  </si>
+  <si>
+    <t>J2_h</t>
+  </si>
+  <si>
+    <t>J3_h</t>
+  </si>
+  <si>
+    <t>0xE1</t>
+  </si>
+  <si>
+    <t>0xE2</t>
   </si>
 </sst>
 </file>
@@ -339,7 +364,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -352,8 +377,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="13">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -501,11 +532,40 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -570,49 +630,73 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -929,8 +1013,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA521C99-CB82-014E-905E-D1830F903609}">
   <dimension ref="B4:AD18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P3" zoomScale="200" workbookViewId="0">
-      <selection activeCell="AC11" sqref="AC11"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -948,12 +1032,12 @@
   <sheetData>
     <row r="4" spans="2:30" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="2:30" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>0</v>
@@ -964,22 +1048,22 @@
       <c r="E5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="30" t="s">
+      <c r="F5" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="30"/>
-      <c r="H5" s="30"/>
-      <c r="I5" s="30"/>
-      <c r="J5" s="30"/>
-      <c r="K5" s="30"/>
-      <c r="L5" s="30"/>
-      <c r="M5" s="30"/>
-      <c r="N5" s="30"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="33"/>
+      <c r="I5" s="33"/>
+      <c r="J5" s="33"/>
+      <c r="K5" s="33"/>
+      <c r="L5" s="33"/>
+      <c r="M5" s="33"/>
+      <c r="N5" s="33"/>
       <c r="O5" s="3" t="s">
         <v>4</v>
       </c>
       <c r="R5" s="17" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="2:30" x14ac:dyDescent="0.2">
@@ -1007,23 +1091,23 @@
       <c r="O6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="R6" s="35"/>
-      <c r="S6" s="34" t="s">
-        <v>64</v>
-      </c>
-      <c r="T6" s="34"/>
-      <c r="U6" s="34"/>
-      <c r="V6" s="34"/>
-      <c r="W6" s="34"/>
-      <c r="X6" s="34"/>
-      <c r="Y6" s="34"/>
-      <c r="Z6" s="34"/>
-      <c r="AA6" s="24" t="s">
-        <v>88</v>
-      </c>
-      <c r="AB6" s="25"/>
-      <c r="AC6" s="25"/>
-      <c r="AD6" s="26"/>
+      <c r="R6" s="37"/>
+      <c r="S6" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="T6" s="26"/>
+      <c r="U6" s="26"/>
+      <c r="V6" s="26"/>
+      <c r="W6" s="26"/>
+      <c r="X6" s="26"/>
+      <c r="Y6" s="26"/>
+      <c r="Z6" s="26"/>
+      <c r="AA6" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="AB6" s="28"/>
+      <c r="AC6" s="28"/>
+      <c r="AD6" s="29"/>
     </row>
     <row r="7" spans="2:30" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
@@ -1052,7 +1136,7 @@
       <c r="M7" s="11"/>
       <c r="N7" s="12"/>
       <c r="O7" s="5"/>
-      <c r="R7" s="36"/>
+      <c r="R7" s="38"/>
       <c r="S7" s="1">
         <v>1</v>
       </c>
@@ -1077,10 +1161,10 @@
       <c r="Z7" s="1">
         <v>8</v>
       </c>
-      <c r="AA7" s="27"/>
-      <c r="AB7" s="28"/>
-      <c r="AC7" s="28"/>
-      <c r="AD7" s="29"/>
+      <c r="AA7" s="30"/>
+      <c r="AB7" s="31"/>
+      <c r="AC7" s="31"/>
+      <c r="AD7" s="32"/>
     </row>
     <row r="8" spans="2:30" x14ac:dyDescent="0.2">
       <c r="B8" s="3" t="s">
@@ -1110,7 +1194,7 @@
       <c r="N8" s="9"/>
       <c r="O8" s="5"/>
       <c r="R8" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="S8" s="1">
         <v>1</v>
@@ -1125,22 +1209,22 @@
         <v>1</v>
       </c>
       <c r="W8" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="X8" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="Y8" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="Z8" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="X8" s="1" t="s">
+      <c r="AA8" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="Y8" s="1" t="s">
+      <c r="AB8" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="Z8" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="AA8" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="AB8" s="1" t="s">
-        <v>71</v>
       </c>
       <c r="AC8" s="1"/>
       <c r="AD8" s="1"/>
@@ -1185,7 +1269,7 @@
       </c>
       <c r="O9" s="3"/>
       <c r="R9" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="S9" s="1">
         <v>1</v>
@@ -1200,22 +1284,22 @@
         <v>1</v>
       </c>
       <c r="W9" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="X9" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="Y9" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="Z9" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="X9" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="Y9" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="Z9" s="1" t="s">
-        <v>78</v>
-      </c>
       <c r="AA9" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="AB9" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="AC9" s="1"/>
       <c r="AD9" s="1"/>
@@ -1274,17 +1358,17 @@
       <c r="V10" s="1">
         <v>0</v>
       </c>
-      <c r="W10" s="34" t="s">
+      <c r="W10" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="X10" s="34"/>
-      <c r="Y10" s="34"/>
-      <c r="Z10" s="34"/>
+      <c r="X10" s="26"/>
+      <c r="Y10" s="26"/>
+      <c r="Z10" s="26"/>
       <c r="AA10" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="AB10" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="AC10" s="1"/>
       <c r="AD10" s="1"/>
@@ -1331,61 +1415,61 @@
       <c r="V11" s="1">
         <v>0</v>
       </c>
-      <c r="W11" s="38">
+      <c r="W11" s="24">
         <v>0</v>
       </c>
-      <c r="X11" s="38">
+      <c r="X11" s="24">
         <v>0</v>
       </c>
-      <c r="Y11" s="38">
+      <c r="Y11" s="24">
         <v>0</v>
       </c>
-      <c r="Z11" s="38" t="s">
-        <v>72</v>
+      <c r="Z11" s="24" t="s">
+        <v>69</v>
       </c>
       <c r="AA11" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="AB11" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="AC11" s="1"/>
     </row>
     <row r="12" spans="2:30" x14ac:dyDescent="0.2">
-      <c r="B12" s="31"/>
-      <c r="C12" s="32"/>
-      <c r="D12" s="32"/>
-      <c r="E12" s="32"/>
-      <c r="F12" s="32"/>
-      <c r="G12" s="32"/>
-      <c r="H12" s="25"/>
-      <c r="I12" s="25"/>
-      <c r="J12" s="25"/>
-      <c r="K12" s="25"/>
-      <c r="L12" s="25"/>
-      <c r="M12" s="25"/>
-      <c r="N12" s="25"/>
-      <c r="O12" s="33"/>
+      <c r="B12" s="34"/>
+      <c r="C12" s="35"/>
+      <c r="D12" s="35"/>
+      <c r="E12" s="35"/>
+      <c r="F12" s="35"/>
+      <c r="G12" s="35"/>
+      <c r="H12" s="28"/>
+      <c r="I12" s="28"/>
+      <c r="J12" s="28"/>
+      <c r="K12" s="28"/>
+      <c r="L12" s="28"/>
+      <c r="M12" s="28"/>
+      <c r="N12" s="28"/>
+      <c r="O12" s="36"/>
       <c r="R12" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="S12" s="34" t="s">
-        <v>66</v>
-      </c>
-      <c r="T12" s="34"/>
-      <c r="U12" s="34"/>
-      <c r="V12" s="34"/>
-      <c r="W12" s="34" t="s">
-        <v>67</v>
-      </c>
-      <c r="X12" s="34"/>
-      <c r="Y12" s="34"/>
-      <c r="Z12" s="34"/>
+      <c r="S12" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="T12" s="26"/>
+      <c r="U12" s="26"/>
+      <c r="V12" s="26"/>
+      <c r="W12" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="X12" s="26"/>
+      <c r="Y12" s="26"/>
+      <c r="Z12" s="26"/>
       <c r="AA12" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="AB12" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="AC12" s="1"/>
       <c r="AD12" s="1"/>
@@ -1399,12 +1483,12 @@
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F13" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="F13" s="43" t="s">
         <v>46</v>
       </c>
-      <c r="G13" s="4" t="s">
+      <c r="G13" s="44" t="s">
         <v>47</v>
       </c>
       <c r="H13" s="7"/>
@@ -1418,23 +1502,23 @@
       <c r="R13" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="S13" s="34" t="s">
-        <v>66</v>
-      </c>
-      <c r="T13" s="34"/>
-      <c r="U13" s="34"/>
-      <c r="V13" s="34"/>
-      <c r="W13" s="34" t="s">
-        <v>67</v>
-      </c>
-      <c r="X13" s="34"/>
-      <c r="Y13" s="34"/>
-      <c r="Z13" s="34"/>
+      <c r="S13" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="T13" s="26"/>
+      <c r="U13" s="26"/>
+      <c r="V13" s="26"/>
+      <c r="W13" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="X13" s="26"/>
+      <c r="Y13" s="26"/>
+      <c r="Z13" s="26"/>
       <c r="AA13" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="AB13" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="AC13" s="1"/>
       <c r="AD13" s="1"/>
@@ -1446,15 +1530,17 @@
       <c r="C14" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="3"/>
+      <c r="D14" s="3" t="s">
+        <v>12</v>
+      </c>
       <c r="E14" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F14" s="43" t="s">
         <v>49</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="G14" s="44" t="s">
         <v>50</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>51</v>
       </c>
       <c r="H14" s="7"/>
       <c r="I14" s="8"/>
@@ -1467,50 +1553,83 @@
       <c r="R14" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="S14" s="34"/>
-      <c r="T14" s="34"/>
-      <c r="U14" s="34"/>
-      <c r="V14" s="34"/>
-      <c r="W14" s="34"/>
-      <c r="X14" s="34"/>
-      <c r="Y14" s="34"/>
-      <c r="Z14" s="34"/>
+      <c r="S14" s="26"/>
+      <c r="T14" s="26"/>
+      <c r="U14" s="26"/>
+      <c r="V14" s="26"/>
+      <c r="W14" s="26"/>
+      <c r="X14" s="26"/>
+      <c r="Y14" s="26"/>
+      <c r="Z14" s="26"/>
       <c r="AA14" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AB14" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC14" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AD14" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="AB14" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="AC14" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="AD14" s="1" t="s">
+    </row>
+    <row r="15" spans="2:30" x14ac:dyDescent="0.2">
+      <c r="B15" s="39" t="s">
+        <v>91</v>
+      </c>
+      <c r="C15" s="39" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="39" t="s">
+        <v>95</v>
+      </c>
+      <c r="F15" s="45" t="s">
+        <v>32</v>
+      </c>
+      <c r="G15" s="46" t="s">
+        <v>33</v>
+      </c>
+      <c r="H15" s="46" t="s">
+        <v>96</v>
+      </c>
+      <c r="I15" s="46" t="s">
+        <v>34</v>
+      </c>
+      <c r="J15" s="46" t="s">
+        <v>97</v>
+      </c>
+      <c r="K15" s="46" t="s">
+        <v>36</v>
+      </c>
+      <c r="L15" s="46" t="s">
+        <v>37</v>
+      </c>
+      <c r="M15" s="46" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B17" s="25" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B17" s="37" t="s">
-        <v>90</v>
-      </c>
-      <c r="C17" s="37"/>
-      <c r="D17" s="37"/>
-      <c r="E17" s="37"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="25"/>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B18" s="37" t="s">
-        <v>91</v>
-      </c>
-      <c r="C18" s="37"/>
-      <c r="D18" s="37"/>
-      <c r="E18" s="37"/>
+      <c r="B18" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="C18" s="25"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="S13:V13"/>
-    <mergeCell ref="W13:Z13"/>
-    <mergeCell ref="S14:Z14"/>
     <mergeCell ref="AA6:AD7"/>
     <mergeCell ref="F5:N5"/>
     <mergeCell ref="B12:O12"/>
@@ -1519,6 +1638,11 @@
     <mergeCell ref="S12:V12"/>
     <mergeCell ref="W12:Z12"/>
     <mergeCell ref="R6:R7"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="S13:V13"/>
+    <mergeCell ref="W13:Z13"/>
+    <mergeCell ref="S14:Z14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1528,8 +1652,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BB565AE-13CD-0640-BA57-0044457625A5}">
   <dimension ref="B3:O18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1540,7 +1664,7 @@
   <sheetData>
     <row r="3" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B3" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C3" s="22"/>
       <c r="D3" s="22"/>
@@ -1554,7 +1678,7 @@
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B4" s="16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C4" s="23" t="s">
         <v>0</v>
@@ -1577,7 +1701,7 @@
         <v>7</v>
       </c>
       <c r="E5" s="23" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.2">
@@ -1591,7 +1715,7 @@
         <v>7</v>
       </c>
       <c r="E6" s="23" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.2">
@@ -1605,7 +1729,7 @@
         <v>7</v>
       </c>
       <c r="E7" s="18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.2">
@@ -1619,7 +1743,7 @@
         <v>7</v>
       </c>
       <c r="E8" s="18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.2">
@@ -1633,7 +1757,7 @@
         <v>7</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.2">
@@ -1647,7 +1771,7 @@
         <v>7</v>
       </c>
       <c r="E10" s="18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.2">
@@ -1667,7 +1791,7 @@
         <v>7</v>
       </c>
       <c r="E12" s="18" t="s">
-        <v>6</v>
+        <v>92</v>
       </c>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.2">
@@ -1681,12 +1805,26 @@
         <v>7</v>
       </c>
       <c r="E13" s="18" t="s">
-        <v>49</v>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B14" s="40" t="s">
+        <v>93</v>
+      </c>
+      <c r="C14" s="42" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="42" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="41" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B15" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C15" s="22"/>
       <c r="D15" s="22"/>
@@ -1694,7 +1832,7 @@
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B16" s="16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C16" s="23" t="s">
         <v>0</v>
@@ -1708,7 +1846,7 @@
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B17" s="16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C17" s="23" t="s">
         <v>6</v>
@@ -1717,12 +1855,12 @@
         <v>7</v>
       </c>
       <c r="E17" s="23" t="s">
-        <v>62</v>
+        <v>98</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B18" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C18" s="23" t="s">
         <v>6</v>
@@ -1731,7 +1869,7 @@
         <v>7</v>
       </c>
       <c r="E18" s="23" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>